<commit_message>
CELERY BASE IS CREATED.. NEED TO CHANGE IN MACBOOK
</commit_message>
<xml_diff>
--- a/media/BAJAJ-PL/Billing/MAR 22/BAJAJ-PL Billing MIS.xlsx
+++ b/media/BAJAJ-PL/Billing/MAR 22/BAJAJ-PL Billing MIS.xlsx
@@ -460,7 +460,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>34380.15</v>
+        <v>46044.75</v>
       </c>
     </row>
     <row r="3">
@@ -473,7 +473,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>18774.88</v>
+        <v>29621.28</v>
       </c>
     </row>
     <row r="4">
@@ -486,7 +486,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2675.97</v>
+        <v>5486.24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CELERY TASK BAR COLORED BASE IS CREATED.. NEED TO CHANGE IN MACBOOK
</commit_message>
<xml_diff>
--- a/media/BAJAJ-PL/Billing/MAR 22/BAJAJ-PL Billing MIS.xlsx
+++ b/media/BAJAJ-PL/Billing/MAR 22/BAJAJ-PL Billing MIS.xlsx
@@ -460,7 +460,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>46044.75</v>
+        <v>1484.1</v>
       </c>
     </row>
     <row r="3">
@@ -473,7 +473,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>29621.28</v>
+        <v>2866.4</v>
       </c>
     </row>
     <row r="4">
@@ -486,7 +486,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>5486.24</v>
+        <v>989.91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>